<commit_message>
Fix 15 but need to find a way d424360f774aed3202766f339ea46d67711a2a8a
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-09T16:21:14+00:00</t>
+    <t>2025-01-11T17:10:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -559,7 +559,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -622,9 +622,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
@@ -635,15 +633,13 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>40</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -662,29 +658,42 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Fix du fix issue#70 198de457108245ea2217d42adc1b60536ebd8ed0
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="108">
   <si>
     <t>Property</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-13T15:32:59+00:00</t>
+    <t>2025-02-16T15:11:19+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -866,7 +866,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -960,30 +960,41 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>97</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
essai fix profil MedReq 28cb65a6ab863847a519515c160d670cb09afb77
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-medicationrequest-conceptmap.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="111">
   <si>
     <t>Property</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-24T15:43:49+00:00</t>
+    <t>2025-04-25T13:21:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>MedicationRequest.priority</t>
+  </si>
+  <si>
+    <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Fourniture</t>
+  </si>
+  <si>
+    <t>MedicationRequest.medication[x].extension.valueBoolean</t>
   </si>
   <si>
     <t>Messages/M_prescription_médicaments/Prescription/Elément_prescr_médic/Id_prescripteur</t>
@@ -665,7 +671,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -721,7 +727,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -734,7 +740,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -747,7 +753,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -760,7 +766,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -773,7 +779,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -786,7 +792,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -799,7 +805,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -812,7 +818,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -825,7 +831,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -838,7 +844,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -851,7 +857,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -907,14 +913,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -925,7 +931,7 @@
         <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -936,7 +942,7 @@
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -947,7 +953,7 @@
         <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -958,7 +964,7 @@
         <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -969,26 +975,26 @@
         <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -1044,27 +1050,27 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>46</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>46</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -1113,14 +1119,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>46</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1212,14 +1218,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>46</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1268,14 +1274,14 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>46</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1692,7 +1698,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1799,7 +1805,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>66</v>
@@ -1815,9 +1821,22 @@
         <v>46</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1864,53 +1883,53 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1959,33 +1978,33 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -2041,75 +2060,75 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E8" s="2"/>
     </row>

</xml_diff>